<commit_message>
fixed the excel file
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/importerProfesseurs.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/importerProfesseurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mini projets\GestionDesAbsencesMigration\GestionDesAbsencesMigration\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC503C7C-5F2B-43CC-98BE-7968C6EE1523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4B5711-6F32-4346-9EAC-5898D69529EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,6 +33,9 @@
     <t>Prenom</t>
   </si>
   <si>
+    <t>Code</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -42,6 +45,9 @@
     <t>prenom1</t>
   </si>
   <si>
+    <t>FF123456</t>
+  </si>
+  <si>
     <t>profmail1@gmail.com</t>
   </si>
   <si>
@@ -51,119 +57,113 @@
     <t>prenom2</t>
   </si>
   <si>
+    <t>FF123457</t>
+  </si>
+  <si>
+    <t>profmail2@gmail.com</t>
+  </si>
+  <si>
     <t>nom3</t>
   </si>
   <si>
     <t>prenom3</t>
   </si>
   <si>
+    <t>FF123458</t>
+  </si>
+  <si>
+    <t>profmail3@gmail.com</t>
+  </si>
+  <si>
     <t>nom4</t>
   </si>
   <si>
     <t>prenom4</t>
   </si>
   <si>
+    <t>FF123459</t>
+  </si>
+  <si>
+    <t>profmail4@gmail.com</t>
+  </si>
+  <si>
     <t>nom5</t>
   </si>
   <si>
     <t>prenom5</t>
   </si>
   <si>
+    <t>FF123460</t>
+  </si>
+  <si>
+    <t>profmail5@gmail.com</t>
+  </si>
+  <si>
     <t>nom6</t>
   </si>
   <si>
     <t>prenom6</t>
   </si>
   <si>
+    <t>FF123461</t>
+  </si>
+  <si>
+    <t>profmail6@gmail.com</t>
+  </si>
+  <si>
     <t>nom7</t>
   </si>
   <si>
     <t>prenom7</t>
   </si>
   <si>
+    <t>FF123462</t>
+  </si>
+  <si>
+    <t>profmail7@gmail.com</t>
+  </si>
+  <si>
     <t>nom8</t>
   </si>
   <si>
     <t>prenom8</t>
   </si>
   <si>
+    <t>FF123463</t>
+  </si>
+  <si>
+    <t>profmail8@gmail.com</t>
+  </si>
+  <si>
     <t>nom9</t>
   </si>
   <si>
     <t>prenom9</t>
   </si>
   <si>
+    <t>FF123464</t>
+  </si>
+  <si>
+    <t>profmail9@gmail.com</t>
+  </si>
+  <si>
     <t>nom10</t>
   </si>
   <si>
     <t>prenom10</t>
   </si>
   <si>
-    <t>profmail2@gmail.com</t>
-  </si>
-  <si>
-    <t>profmail3@gmail.com</t>
-  </si>
-  <si>
-    <t>profmail4@gmail.com</t>
-  </si>
-  <si>
-    <t>profmail5@gmail.com</t>
-  </si>
-  <si>
-    <t>profmail6@gmail.com</t>
-  </si>
-  <si>
-    <t>profmail7@gmail.com</t>
-  </si>
-  <si>
-    <t>profmail8@gmail.com</t>
-  </si>
-  <si>
-    <t>profmail9@gmail.com</t>
+    <t>FF123465</t>
   </si>
   <si>
     <t>profmail10@gmail.com</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>FF123456</t>
-  </si>
-  <si>
-    <t>FF123457</t>
-  </si>
-  <si>
-    <t>FF123458</t>
-  </si>
-  <si>
-    <t>FF123459</t>
-  </si>
-  <si>
-    <t>FF123460</t>
-  </si>
-  <si>
-    <t>FF123461</t>
-  </si>
-  <si>
-    <t>FF123462</t>
-  </si>
-  <si>
-    <t>FF123463</t>
-  </si>
-  <si>
-    <t>FF123464</t>
-  </si>
-  <si>
-    <t>FF123465</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,12 +175,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,7 +201,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -491,202 +486,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E6:H21"/>
+  <dimension ref="D5:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="G13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="G14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="E15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="G15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1" xr:uid="{73D5147B-F275-4FE3-8557-AF610AECAB89}"/>
-    <hyperlink ref="H8" r:id="rId2" xr:uid="{4BB85093-4A31-421A-997E-40ED591579BC}"/>
-    <hyperlink ref="H9" r:id="rId3" xr:uid="{A8DE55A5-ADC1-4FF9-AC74-4E13DB119311}"/>
-    <hyperlink ref="H10" r:id="rId4" xr:uid="{99F44063-A73A-497C-865A-DD43E659633C}"/>
-    <hyperlink ref="H11" r:id="rId5" xr:uid="{4283BFA2-4778-459A-8B76-7AB3D425C8CA}"/>
-    <hyperlink ref="H12" r:id="rId6" xr:uid="{07FB5619-925D-4AC9-9E7A-DA48CA2561C0}"/>
-    <hyperlink ref="H13" r:id="rId7" xr:uid="{4186F4A3-B55C-417A-AC20-50D5D8CEAE82}"/>
-    <hyperlink ref="H14" r:id="rId8" xr:uid="{D1904048-42E5-4C49-9E0A-359B9BCF9C51}"/>
-    <hyperlink ref="H15" r:id="rId9" xr:uid="{8EF6E234-175E-4BF8-88F3-976D3E0B0912}"/>
-    <hyperlink ref="H16" r:id="rId10" xr:uid="{F5927B7D-E995-4F04-8165-2672910198CA}"/>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{73D5147B-F275-4FE3-8557-AF610AECAB89}"/>
+    <hyperlink ref="G7" r:id="rId2" xr:uid="{4BB85093-4A31-421A-997E-40ED591579BC}"/>
+    <hyperlink ref="G8" r:id="rId3" xr:uid="{A8DE55A5-ADC1-4FF9-AC74-4E13DB119311}"/>
+    <hyperlink ref="G9" r:id="rId4" xr:uid="{99F44063-A73A-497C-865A-DD43E659633C}"/>
+    <hyperlink ref="G10" r:id="rId5" xr:uid="{4283BFA2-4778-459A-8B76-7AB3D425C8CA}"/>
+    <hyperlink ref="G11" r:id="rId6" xr:uid="{07FB5619-925D-4AC9-9E7A-DA48CA2561C0}"/>
+    <hyperlink ref="G12" r:id="rId7" xr:uid="{4186F4A3-B55C-417A-AC20-50D5D8CEAE82}"/>
+    <hyperlink ref="G13" r:id="rId8" xr:uid="{D1904048-42E5-4C49-9E0A-359B9BCF9C51}"/>
+    <hyperlink ref="G14" r:id="rId9" xr:uid="{8EF6E234-175E-4BF8-88F3-976D3E0B0912}"/>
+    <hyperlink ref="G15" r:id="rId10" xr:uid="{F5927B7D-E995-4F04-8165-2672910198CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change code prof to cne
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/importerProfesseurs.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/importerProfesseurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mini projets\GestionDesAbsencesMigration\GestionDesAbsencesMigration\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4B5711-6F32-4346-9EAC-5898D69529EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B935BDD1-F5A0-451E-8853-92AF96206EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>Prenom</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>profmail10@gmail.com</t>
+  </si>
+  <si>
+    <t>CNE</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="D5:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,150 +505,150 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed prof password while importing from excel
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/importerProfesseurs.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/importerProfesseurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mini projets\GestionDesAbsencesMigration\GestionDesAbsencesMigration\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B935BDD1-F5A0-451E-8853-92AF96206EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BDF731-2FF7-4D1D-8F15-36AD6DE32629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,7 +156,7 @@
     <t>profmail10@gmail.com</t>
   </si>
   <si>
-    <t>CNE</t>
+    <t>CIN</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="D5:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>